<commit_message>
Test and add demo files
</commit_message>
<xml_diff>
--- a/test-files/tests/xlsx/expected-four-fill.xlsx
+++ b/test-files/tests/xlsx/expected-four-fill.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\sethg\Documents\CS-321\Project\Implementation\pdf-manager\test-files\tests\xlsx\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{02AFC09A-F709-4117-87F2-A749A2BB27BE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4012EB5D-E934-441E-9D3B-546637D3B0A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3444" yWindow="2196" windowWidth="15708" windowHeight="11016" xr2:uid="{C54177E3-FD80-4461-976C-50F0D511DF18}"/>
+    <workbookView xWindow="3444" yWindow="1944" windowWidth="15708" windowHeight="11016" xr2:uid="{C54177E3-FD80-4461-976C-50F0D511DF18}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -36,15 +36,9 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
-    <t>First Name</t>
-  </si>
-  <si>
     <t>Ace</t>
   </si>
   <si>
-    <t>Last Name</t>
-  </si>
-  <si>
     <t>Valentine</t>
   </si>
   <si>
@@ -58,6 +52,12 @@
   </si>
   <si>
     <t>true.love.is.real@gmail.com</t>
+  </si>
+  <si>
+    <t>FirstName[0]</t>
+  </si>
+  <si>
+    <t>LastName[0]</t>
   </si>
 </sst>
 </file>
@@ -423,41 +423,41 @@
   <dimension ref="A1:B4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E3" sqref="E3"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B1" t="s">
         <v>0</v>
-      </c>
-      <c r="B1" t="s">
-        <v>1</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
-        <v>2</v>
+        <v>7</v>
       </c>
       <c r="B2" t="s">
-        <v>3</v>
+        <v>1</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
-        <v>4</v>
+        <v>2</v>
       </c>
       <c r="B3" t="s">
-        <v>5</v>
+        <v>3</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
-        <v>6</v>
+        <v>4</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>7</v>
+        <v>5</v>
       </c>
     </row>
   </sheetData>

</xml_diff>